<commit_message>
Added Goto SubNavBar Using Text Function
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_Digisales/SCD0174 - Penambahan Kriteria Lead yang ada di Store, termasuk Free, Dedicated, Kelolaan dan Prospek.xlsx
+++ b/Lib_Repo_Excel/FileExcel_Digisales/SCD0174 - Penambahan Kriteria Lead yang ada di Store, termasuk Free, Dedicated, Kelolaan dan Prospek.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1442\Desktop\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29138A78-BA8A-4086-A3CF-65248F61B8FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40856FDD-0DA0-4E83-AE28-E838D9DD6380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1680" yWindow="3630" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SCD0174" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>RUN</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>QUERY1</t>
+  </si>
+  <si>
+    <t>Prospek</t>
   </si>
 </sst>
 </file>
@@ -515,8 +518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0EAF5E5-8229-45B3-AC11-8AED029F52F4}">
   <dimension ref="A1:V6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,9 +604,7 @@
       </c>
     </row>
     <row r="2" spans="1:22" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>0</v>
-      </c>
+      <c r="A2" s="9"/>
       <c r="B2" s="10" t="s">
         <v>16</v>
       </c>
@@ -665,8 +666,11 @@
       <c r="L3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="M3" t="s">
+      <c r="O3" t="s">
         <v>27</v>
+      </c>
+      <c r="P3" t="s">
+        <v>29</v>
       </c>
       <c r="R3" s="1"/>
       <c r="S3" s="2"/>

</xml_diff>

<commit_message>
Scripting SCD0174 - Penambahan Kriteria Lead yang ada di Store, termasuk Free, Dedicated, Kelolaan dan Prospek penuh bug
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_Digisales/SCD0174 - Penambahan Kriteria Lead yang ada di Store, termasuk Free, Dedicated, Kelolaan dan Prospek.xlsx
+++ b/Lib_Repo_Excel/FileExcel_Digisales/SCD0174 - Penambahan Kriteria Lead yang ada di Store, termasuk Free, Dedicated, Kelolaan dan Prospek.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1442\Desktop\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40856FDD-0DA0-4E83-AE28-E838D9DD6380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D96BD63-C535-47EF-B23E-9395BE96737C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="3630" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SCD0174" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
   <si>
     <t>RUN</t>
   </si>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>NAVBAR_MENU</t>
-  </si>
-  <si>
-    <t>SUB_NAVBAR</t>
   </si>
   <si>
     <t>SUB_SUB_NAVBAR</t>
@@ -99,12 +96,6 @@
     <t>SIDEBAR_MENU</t>
   </si>
   <si>
-    <t>SIDEBAR_SUBMENU</t>
-  </si>
-  <si>
-    <t>SIDEBAR_SUBMENU_SUBMENU</t>
-  </si>
-  <si>
     <t>Upload Data Leads</t>
   </si>
   <si>
@@ -120,7 +111,88 @@
     <t>QUERY1</t>
   </si>
   <si>
-    <t>Prospek</t>
+    <t>Dedicated</t>
+  </si>
+  <si>
+    <t>TEXT4</t>
+  </si>
+  <si>
+    <t>CIF</t>
+  </si>
+  <si>
+    <t>Cek Data Leads Free dan Dedicated</t>
+  </si>
+  <si>
+    <t>1. Login digisales mobile sebagai Sales
+2. Buka Store, Cek data Free dan Dedicated
+3. Cek data pada database</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Data pada Free dan Dedicated sudah muncul
+ - Data yang ada pada database bisa ditampilkan</t>
+  </si>
+  <si>
+    <t>Menambahkan Customer Flagging</t>
+  </si>
+  <si>
+    <t>1. Login digisales mobile sebagai Sales
+2. Search data customer pada Profiling Leads
+3. Add to Flagging pada customer yang dipilih
+4. Ajukan ke penyelia
+5. Cek data pada customer flagging</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Berhasil add to flagging customer
+ - Berhasil mengajukan ke penyelia
+ - Muncul data pada customer flagging dengan status "Menunggu Approval Pemimpin Cabang"</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>select ds.CUST_NAME,z.Npp, ds.BNI_CIF_KEY, z.BranchCode CabangSales, z.KLNCode OutletSales, ds.BRANCH_CODE CabangNasabah, ds.KLN_CODE OutletNasabah,
+ds.DPK, ds.TABUNGAN, ds.CUST_TYPE from Digisales_KPI..DPK_SEGMENTASI ds
+join +(9)select a.Npp, d.Code BranchCode, d.KodeEIS KLNCode, d.KodeWilayah from DigisalesNew..Tbl_Pegawai a
+join +(9)SELECT b.Id, b.Code, b.KodeEIS, c.NamaWilayah, c.Code KodeWilayah FROM  DigisalesNew..Tbl_Unit b 
+join DigisalesNew..Tbl_Unit_Wilayah c on b.Wilayah_Id = c.Id +(0) d on a.Unit_Id = d.Id +(0)z 
+on ds.BRANCH_CODE = z.BranchCode 
+where z.Npp in +(9)22914+(0) and ds.BNI_CIF_KEY IN +(9)'9709520792.0000','9821041813.0000'+(0)</t>
+  </si>
+  <si>
+    <t>QUERY2</t>
+  </si>
+  <si>
+    <t>QUERY3</t>
+  </si>
+  <si>
+    <t>EXPL_QUERY1</t>
+  </si>
+  <si>
+    <t>EXPL_QUERY2</t>
+  </si>
+  <si>
+    <t>EXPL_QUERY3</t>
+  </si>
+  <si>
+    <t>Pembuktian Data Leads pada Database</t>
+  </si>
+  <si>
+    <t>HOSTNAME</t>
+  </si>
+  <si>
+    <t>USER_DB</t>
+  </si>
+  <si>
+    <t>PASSWORD_DB</t>
+  </si>
+  <si>
+    <t>sa</t>
+  </si>
+  <si>
+    <t>4eFfEJAA!</t>
+  </si>
+  <si>
+    <t>192.168.232.6</t>
   </si>
 </sst>
 </file>
@@ -186,9 +258,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -209,6 +278,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -516,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0EAF5E5-8229-45B3-AC11-8AED029F52F4}">
-  <dimension ref="A1:V6"/>
+  <dimension ref="A1:X6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" topLeftCell="E4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,19 +607,20 @@
     <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="25" customWidth="1"/>
-    <col min="19" max="19" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="23.42578125" customWidth="1"/>
-    <col min="21" max="21" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.85546875" customWidth="1"/>
+    <col min="17" max="17" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -573,126 +646,193 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J1" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="K1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="L1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="M1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="N1" t="s">
         <v>14</v>
       </c>
       <c r="O1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="P1" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="Q1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R1" t="s">
+        <v>38</v>
+      </c>
+      <c r="S1" t="s">
+        <v>39</v>
+      </c>
+      <c r="T1" t="s">
+        <v>40</v>
+      </c>
+      <c r="U1" t="s">
+        <v>41</v>
+      </c>
+      <c r="V1" t="s">
+        <v>43</v>
+      </c>
+      <c r="W1" t="s">
+        <v>44</v>
+      </c>
+      <c r="X1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="R1" t="s">
+      <c r="C2" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="11">
+        <v>52326</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="12"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="13"/>
+      <c r="U2" s="7"/>
+    </row>
+    <row r="3" spans="1:24" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="11">
+        <v>22914</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="8"/>
+      <c r="J3" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="8"/>
+      <c r="N3" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="P3" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q3" s="12"/>
+      <c r="S3" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="U3" s="2"/>
+      <c r="V3" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="W3" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="X3" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="11">
+        <v>22914</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="L4" s="8">
+        <v>9821041813</v>
+      </c>
+      <c r="M4" s="8" t="s">
         <v>28</v>
       </c>
+      <c r="T4" s="1"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="2"/>
     </row>
-    <row r="2" spans="1:22" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
-      <c r="B2" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="12">
-        <v>52326</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="14"/>
-      <c r="S2" s="8"/>
-      <c r="U2" s="8"/>
-      <c r="V2" s="8"/>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="5">
-        <v>22914</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" t="s">
-        <v>11</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="O3" t="s">
-        <v>27</v>
-      </c>
-      <c r="P3" t="s">
-        <v>29</v>
-      </c>
-      <c r="R3" s="1"/>
-      <c r="S3" s="2"/>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B4" s="4"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="6"/>
-      <c r="L4" s="3"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="2"/>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B5" s="4"/>
       <c r="F5" s="5"/>
       <c r="G5" s="6"/>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
       <c r="F6" s="5"/>
       <c r="G6" s="6"/>

</xml_diff>